<commit_message>
Erste Arbeiten an SP 'insert mitarbeiter'. Datenfluss von Excel bis Datenbank steht rudimentär.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418601F8-2B14-45BA-9913-5ECD7E2E7C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D737F30-91BE-46A6-8A90-DE9988F1E51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>maennlich</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -39,9 +36,6 @@
     <t>DE00 0000 0000 0000 0000 00</t>
   </si>
   <si>
-    <t>0175 2572025</t>
-  </si>
-  <si>
     <t>Daten</t>
   </si>
   <si>
@@ -51,46 +45,88 @@
     <t>maxmustermann@web.de</t>
   </si>
   <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>Steuernummer</t>
+  </si>
+  <si>
+    <t>Sozialversicherungsnummer</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Mustermann</t>
+  </si>
+  <si>
+    <t>Zweitname</t>
+  </si>
+  <si>
+    <t>0175 1234567</t>
+  </si>
+  <si>
+    <t>Strasse</t>
+  </si>
+  <si>
+    <t>Musterstraße</t>
+  </si>
+  <si>
+    <t>Hausnummer</t>
+  </si>
+  <si>
+    <t>Postleitzahl</t>
+  </si>
+  <si>
+    <t>Stadt</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Deutschland</t>
+  </si>
+  <si>
+    <t>private Telefonnummer</t>
+  </si>
+  <si>
+    <t>private E-Mail</t>
+  </si>
+  <si>
+    <t>dienstliche Telefonnummer</t>
+  </si>
+  <si>
+    <t>030 987654321</t>
+  </si>
+  <si>
+    <t>dienstliche E-Mail</t>
+  </si>
+  <si>
+    <t>Mustermann@testfirma.de</t>
+  </si>
+  <si>
+    <t>Geburtsdatum</t>
+  </si>
+  <si>
+    <t>Eintrittsdatum</t>
+  </si>
+  <si>
     <t>12.12.1992</t>
   </si>
   <si>
-    <t>01.12.2023</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Nachname</t>
-  </si>
-  <si>
-    <t>Geschlecht</t>
-  </si>
-  <si>
-    <t>Geburtsdatum</t>
-  </si>
-  <si>
-    <t>Eintrittsdatum</t>
-  </si>
-  <si>
-    <t>Steuernummer</t>
-  </si>
-  <si>
-    <t>Sozialversicherungsnummer</t>
-  </si>
-  <si>
-    <t>IBAN</t>
-  </si>
-  <si>
-    <t>Telefonnummer</t>
-  </si>
-  <si>
-    <t>E-Mail</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Mustermann</t>
+    <t>Austrittsdatum</t>
   </si>
 </sst>
 </file>
@@ -122,12 +158,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,11 +191,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -429,9 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -441,96 +494,159 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6">
+        <v>12358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{CFA18DE6-0AED-4D2D-8B09-CFE58AEA95B1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mitarbeiter haben nun Attribut 'Personalnummer'. ST-Funktionen 'insert_tbl_mitarbeiter' und 'pruefe_einmaligkeit_personalnummer' erfolgreich implementiert und funktioniert so wie beabsichtigt.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D737F30-91BE-46A6-8A90-DE9988F1E51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A989F45-308B-4C6F-A31E-F240F46622B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Austrittsdatum</t>
+  </si>
+  <si>
+    <t>Personalnummer</t>
+  </si>
+  <si>
+    <t>M100001</t>
   </si>
 </sst>
 </file>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,137 +508,137 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="6">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="6">
-        <v>12358</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B18" s="6">
+        <v>12358</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>20</v>
@@ -640,9 +646,17 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Funktion 'insert_neuer_mitarbeiter' überarbeitet. Funktion 'test_set_up' erstellt und in die Unittest-Klassen implementiert. Alle Funktionen laufen wie erwartet.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A989F45-308B-4C6F-A31E-F240F46622B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD5E8A-9212-4219-A7AC-49BCF3956730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -133,6 +133,81 @@
   </si>
   <si>
     <t>M100001</t>
+  </si>
+  <si>
+    <t>01.01.2024</t>
+  </si>
+  <si>
+    <t>Geschlecht</t>
+  </si>
+  <si>
+    <t>Mitarbeitertyp</t>
+  </si>
+  <si>
+    <t>Gesellschaft</t>
+  </si>
+  <si>
+    <t>Jobtitel</t>
+  </si>
+  <si>
+    <t>Erfahrungsstufe</t>
+  </si>
+  <si>
+    <t>Abteilung</t>
+  </si>
+  <si>
+    <t>Wochenarbeitszeit</t>
+  </si>
+  <si>
+    <t>Steuerklasse</t>
+  </si>
+  <si>
+    <t>Tarif</t>
+  </si>
+  <si>
+    <t>AT-Grundgehalt</t>
+  </si>
+  <si>
+    <t>AT-Weihnachtsgeld</t>
+  </si>
+  <si>
+    <t>AT-Urlaubsgeld</t>
+  </si>
+  <si>
+    <t>Zuschuss privater Zusatzbeitrag</t>
+  </si>
+  <si>
+    <t>Zuschuss private Pflegeversicheurng</t>
+  </si>
+  <si>
+    <t>Zuschuss private Krankenversicherung</t>
+  </si>
+  <si>
+    <t>wohnhaft Sachsen?</t>
+  </si>
+  <si>
+    <t>gesetzlich versichert?</t>
+  </si>
+  <si>
+    <t>privat versichert?</t>
+  </si>
+  <si>
+    <t>aussertariflich beschaeftigt?</t>
+  </si>
+  <si>
+    <t>Tarifbeschaeftigt?</t>
+  </si>
+  <si>
+    <t>unfallversichert?</t>
+  </si>
+  <si>
+    <t>rentenversichert?</t>
+  </si>
+  <si>
+    <t>Mitglied gesetzliche Krankenkasse (Abkürzung)</t>
+  </si>
+  <si>
+    <t>Mitglied gesetzliche Krankenkasse (vollständiger Name)</t>
   </si>
 </sst>
 </file>
@@ -164,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +258,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -197,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -205,6 +298,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -486,15 +583,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -548,7 +645,9 @@
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -659,6 +758,153 @@
       <c r="B21" s="6" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="8"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="9"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Methoden '_existenz_str_daten_feststellen' und '_existenz_date_daten_feststellen'erzeugt.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD5E8A-9212-4219-A7AC-49BCF3956730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A213A86F-C5F5-482F-82A4-9EE1242ACFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -301,7 +301,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -583,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,9 +902,6 @@
       </c>
       <c r="B45" s="7"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Neue Tests erstellt. Test 'test_nutzer_aus_Nutzerliste_entfernen'funktioniert aus unbekannten Gründen noch nicht. Ansonsten sind alle Methoden der Klassen 'Mandant' und 'Nutzer' nun ausgetestet. Ausnahme: Methode 'abfrage_ausfuehren' aus Klasse 'Nutzer'. Dies kommt erst am Ende.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A213A86F-C5F5-482F-82A4-9EE1242ACFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02E4FB1-75AF-478F-A43C-EB2EAFE8FAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
in Den SP-Funktionen, die sich mit der Erstellung und Entfernung von Mandanten und Nutzern befassen, Code für die Umstellung des current_tenant implementiert.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02E4FB1-75AF-478F-A43C-EB2EAFE8FAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10519056-800F-4BD8-A185-3C5097E514BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Bereiche Geschlechter und Mitarbeitertypen hinzugefügt. Alle 42 Tests laufen. Datenimport läuft soweit ebenfalls.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10519056-800F-4BD8-A185-3C5097E514BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01A536D-A7A9-4034-BD62-8E041FCEED3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -60,12 +60,6 @@
     <t>IBAN</t>
   </si>
   <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Mustermann</t>
-  </si>
-  <si>
     <t>Zweitname</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>Stadt</t>
   </si>
   <si>
-    <t>Berlin</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -208,6 +199,24 @@
   </si>
   <si>
     <t>Mitglied gesetzliche Krankenkasse (vollständiger Name)</t>
+  </si>
+  <si>
+    <t>Bernau</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Musterfrau</t>
+  </si>
+  <si>
+    <t>Erika</t>
+  </si>
+  <si>
+    <t>weiblich</t>
+  </si>
+  <si>
+    <t>Werkstudent</t>
   </si>
 </sst>
 </file>
@@ -239,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,12 +285,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -290,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -301,6 +340,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -582,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,7 +638,7 @@
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -602,307 +646,360 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="B17" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="6">
         <v>12358</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="7"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="B25" s="2"/>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="B26" s="2"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="9"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="B27" s="5"/>
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="B28" s="7"/>
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="B29" s="8"/>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="B31" s="9"/>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="B33" s="2"/>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="8"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="B34" s="2"/>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="9"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="9"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="5"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="B43" s="7"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="5"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="5"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B41" s="5"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="7"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="7"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="7"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="B45" s="7"/>
+      <c r="D45" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{71AFB16E-529B-4436-B8EE-EE56A3A5D5CA}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{37BFBA39-2674-4F74-BA9A-74B241690977}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bereich 'Entgelt' in Datenbank eingefügt. Alle Tests laufen, außer Tear Down bei test_tbl_geschlechter macht Probleme.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847773D-5D4A-407B-9330-6383B4AE8F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1D6BDD-8D4A-4D97-9B1D-10A381CDB9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -184,9 +184,6 @@
     <t>privat versichert?</t>
   </si>
   <si>
-    <t>aussertariflich beschaeftigt?</t>
-  </si>
-  <si>
     <t>Tarifbeschaeftigt?</t>
   </si>
   <si>
@@ -272,6 +269,27 @@
   </si>
   <si>
     <t>Mustermann</t>
+  </si>
+  <si>
+    <t>tarifbeschaeftigt</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Grundgehalt</t>
+  </si>
+  <si>
+    <t>Weihnachtsgeld</t>
+  </si>
+  <si>
+    <t>Urlaubgeld</t>
+  </si>
+  <si>
+    <t>Gewerkschaft</t>
+  </si>
+  <si>
+    <t>verdi</t>
   </si>
 </sst>
 </file>
@@ -688,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +740,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -738,7 +756,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -862,7 +880,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="10"/>
     </row>
@@ -871,7 +889,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="10"/>
     </row>
@@ -889,7 +907,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="10"/>
     </row>
@@ -898,7 +916,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23" s="10"/>
     </row>
@@ -925,25 +943,25 @@
         <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="D28" s="10"/>
     </row>
@@ -952,7 +970,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="10"/>
     </row>
@@ -961,7 +979,7 @@
         <v>38</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D30" s="10"/>
     </row>
@@ -970,137 +988,170 @@
         <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="13"/>
+        <v>52</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="5"/>
+      <c r="A35" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="9">
+        <v>3523.76</v>
+      </c>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="9">
+        <v>1254.28</v>
+      </c>
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="9">
+        <v>2568.75</v>
+      </c>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="B39" s="5"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+      <c r="B40" s="5"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
+      <c r="B41" s="5"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="D40" s="11"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="15"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="7"/>
+      <c r="A45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="2"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="7"/>
+      <c r="A46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="2"/>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="7"/>
+      <c r="A47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="2"/>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B48" s="7"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B49" s="7"/>
       <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="7"/>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="D52" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1117,7 +1168,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E880C197-BC95-4C5B-A656-6C63E902724E}">
           <x14:formula1>
             <xm:f>Tabelle2!$A$2:$A$4</xm:f>
@@ -1142,6 +1193,12 @@
           </x14:formula1>
           <xm:sqref>B28</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D34A55A2-833F-4BC2-A21D-77C18B0F6333}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$I$2:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B33</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1150,15 +1207,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A41E031-B515-4B55-B38F-F0D31894393C}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1169,65 +1226,74 @@
         <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Vorbereitungen für die Implementation der SV-Tabellen durchgeführt. Excel-Tabelle entsprechend vorbereitet.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1D6BDD-8D4A-4D97-9B1D-10A381CDB9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4B4FC5-2FCB-40DA-B4E4-8A4F41F8D3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -124,172 +124,226 @@
     <t>Personalnummer</t>
   </si>
   <si>
+    <t>01.01.2024</t>
+  </si>
+  <si>
+    <t>Geschlecht</t>
+  </si>
+  <si>
+    <t>Mitarbeitertyp</t>
+  </si>
+  <si>
+    <t>Gesellschaft</t>
+  </si>
+  <si>
+    <t>Jobtitel</t>
+  </si>
+  <si>
+    <t>Erfahrungsstufe</t>
+  </si>
+  <si>
+    <t>Abteilung</t>
+  </si>
+  <si>
+    <t>Wochenarbeitszeit</t>
+  </si>
+  <si>
+    <t>Steuerklasse</t>
+  </si>
+  <si>
+    <t>Tarif</t>
+  </si>
+  <si>
+    <t>Zuschuss privater Zusatzbeitrag</t>
+  </si>
+  <si>
+    <t>Zuschuss private Pflegeversicheurng</t>
+  </si>
+  <si>
+    <t>Zuschuss private Krankenversicherung</t>
+  </si>
+  <si>
+    <t>wohnhaft Sachsen?</t>
+  </si>
+  <si>
+    <t>Tarifbeschaeftigt?</t>
+  </si>
+  <si>
+    <t>unfallversichert?</t>
+  </si>
+  <si>
+    <t>Mitglied gesetzliche Krankenkasse (Abkürzung)</t>
+  </si>
+  <si>
+    <t>Mitglied gesetzliche Krankenkasse (vollständiger Name)</t>
+  </si>
+  <si>
+    <t>Bernau</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>weiblich</t>
+  </si>
+  <si>
+    <t>Werkstudent</t>
+  </si>
+  <si>
+    <t>Personalcontrolling</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Führungskraft</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>maennlich</t>
+  </si>
+  <si>
+    <t>divers</t>
+  </si>
+  <si>
+    <t>Angestellter</t>
+  </si>
+  <si>
+    <t>Arbeiter</t>
+  </si>
+  <si>
+    <t>Auszubildender</t>
+  </si>
+  <si>
+    <t>Praktikant</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>Anzahl Kinder</t>
+  </si>
+  <si>
+    <t>Abkuerzung Abteilung</t>
+  </si>
+  <si>
+    <t>Abkuerzung Gesellschaft</t>
+  </si>
+  <si>
+    <t>Berliner Stadtreinigung</t>
+  </si>
+  <si>
+    <t>BSR</t>
+  </si>
+  <si>
+    <t>Grundgehalt</t>
+  </si>
+  <si>
+    <t>Weihnachtsgeld</t>
+  </si>
+  <si>
+    <t>Urlaubgeld</t>
+  </si>
+  <si>
+    <t>Gewerkschaft</t>
+  </si>
+  <si>
+    <t>verdi</t>
+  </si>
+  <si>
     <t>M100001</t>
   </si>
   <si>
-    <t>01.01.2024</t>
-  </si>
-  <si>
-    <t>Geschlecht</t>
-  </si>
-  <si>
-    <t>Mitarbeitertyp</t>
-  </si>
-  <si>
-    <t>Gesellschaft</t>
-  </si>
-  <si>
-    <t>Jobtitel</t>
-  </si>
-  <si>
-    <t>Erfahrungsstufe</t>
-  </si>
-  <si>
-    <t>Abteilung</t>
-  </si>
-  <si>
-    <t>Wochenarbeitszeit</t>
-  </si>
-  <si>
-    <t>Steuerklasse</t>
-  </si>
-  <si>
-    <t>Tarif</t>
-  </si>
-  <si>
-    <t>AT-Grundgehalt</t>
-  </si>
-  <si>
-    <t>AT-Weihnachtsgeld</t>
-  </si>
-  <si>
-    <t>AT-Urlaubsgeld</t>
-  </si>
-  <si>
-    <t>Zuschuss privater Zusatzbeitrag</t>
-  </si>
-  <si>
-    <t>Zuschuss private Pflegeversicheurng</t>
-  </si>
-  <si>
-    <t>Zuschuss private Krankenversicherung</t>
-  </si>
-  <si>
-    <t>wohnhaft Sachsen?</t>
-  </si>
-  <si>
-    <t>gesetzlich versichert?</t>
-  </si>
-  <si>
-    <t>privat versichert?</t>
-  </si>
-  <si>
-    <t>Tarifbeschaeftigt?</t>
-  </si>
-  <si>
-    <t>unfallversichert?</t>
-  </si>
-  <si>
-    <t>rentenversichert?</t>
-  </si>
-  <si>
-    <t>Mitglied gesetzliche Krankenkasse (Abkürzung)</t>
-  </si>
-  <si>
-    <t>Mitglied gesetzliche Krankenkasse (vollständiger Name)</t>
-  </si>
-  <si>
-    <t>Bernau</t>
-  </si>
-  <si>
-    <t>Brandenburg</t>
-  </si>
-  <si>
-    <t>weiblich</t>
-  </si>
-  <si>
-    <t>Werkstudent</t>
-  </si>
-  <si>
-    <t>Personalcontrolling</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>Führungskraft</t>
-  </si>
-  <si>
-    <t>nein</t>
-  </si>
-  <si>
-    <t>maennlich</t>
-  </si>
-  <si>
-    <t>divers</t>
-  </si>
-  <si>
-    <t>Angestellter</t>
-  </si>
-  <si>
-    <t>Arbeiter</t>
-  </si>
-  <si>
-    <t>Auszubildender</t>
-  </si>
-  <si>
-    <t>Praktikant</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
-    <t>Data Analyst</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>Anzahl Kinder</t>
-  </si>
-  <si>
-    <t>Abkuerzung Abteilung</t>
-  </si>
-  <si>
-    <t>Abkuerzung Gesellschaft</t>
-  </si>
-  <si>
-    <t>Berliner Stadtreinigung</t>
-  </si>
-  <si>
-    <t>BSR</t>
-  </si>
-  <si>
     <t>Max</t>
   </si>
   <si>
     <t>Mustermann</t>
   </si>
   <si>
-    <t>tarifbeschaeftigt</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>Grundgehalt</t>
-  </si>
-  <si>
-    <t>Weihnachtsgeld</t>
-  </si>
-  <si>
-    <t>Urlaubgeld</t>
-  </si>
-  <si>
-    <t>Gewerkschaft</t>
-  </si>
-  <si>
-    <t>verdi</t>
+    <t>gesetzlich krankenversichert?</t>
+  </si>
+  <si>
+    <t>Arbeitslosenversichert?</t>
+  </si>
+  <si>
+    <t>Rentenversichert?</t>
+  </si>
+  <si>
+    <t>AG-Rentenbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>AN-Rentenbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>Beitragsbemessungsgrenze Rente Ost</t>
+  </si>
+  <si>
+    <t>Beitragsbemessungsgrenze Rente West</t>
+  </si>
+  <si>
+    <t>AG-Arbeitslosenversicherungsbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>AN-Arbeitslosenversicherungsbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>Beitragsbemessungsgrenze Arbeitslosenversicherung Ost</t>
+  </si>
+  <si>
+    <t>Beitragsbemessungsgrenze Arbeitslosenversicherung West</t>
+  </si>
+  <si>
+    <t>AG-Unfallversicherungsbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>Risikoklasse Unfallversicherung</t>
+  </si>
+  <si>
+    <t>Zusatzbeitrag Krankenversicherung</t>
+  </si>
+  <si>
+    <t>AG-Krankenversicherungsbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>AN-Krankenversicherungsbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>Beitragsbemessungsgrenze Krankenversicherung Ost</t>
+  </si>
+  <si>
+    <t>Beitragsbemessungsgrenze Krankenversicherung West</t>
+  </si>
+  <si>
+    <t>AN-Pflegeversicherungsbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>Beitragsbemessungsgrenze Pflegeversicherung Ost</t>
+  </si>
+  <si>
+    <t>Beitragsbemessungsgrenze Pflegeversicherung West</t>
+  </si>
+  <si>
+    <t>privat krankenversichert?</t>
+  </si>
+  <si>
+    <t>ja/nein</t>
+  </si>
+  <si>
+    <t>Dualstudent</t>
+  </si>
+  <si>
+    <t>AG-Pflegeversicherungsbeitrag in Prozent</t>
+  </si>
+  <si>
+    <t>A5-1</t>
   </si>
 </sst>
 </file>
@@ -377,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -403,12 +457,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -425,6 +488,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -706,15 +778,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -731,7 +803,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -740,7 +812,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -756,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -774,7 +846,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -880,7 +952,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D19" s="10"/>
     </row>
@@ -889,7 +961,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D20" s="10"/>
     </row>
@@ -904,25 +976,25 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="14">
         <v>1</v>
@@ -931,7 +1003,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="8">
         <v>35</v>
@@ -940,218 +1012,337 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="11"/>
+      <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="11"/>
+        <v>105</v>
+      </c>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B36" s="9">
         <v>3523.76</v>
       </c>
-      <c r="D36" s="11"/>
+      <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B37" s="9">
         <v>1254.28</v>
       </c>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B38" s="9">
         <v>2568.75</v>
       </c>
-      <c r="D38" s="11"/>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="D40" s="11"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="B42" s="2"/>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="18"/>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="18"/>
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="18"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="18"/>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="18"/>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="15"/>
-      <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="B51" s="17"/>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="19"/>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="19"/>
+      <c r="D53" s="11"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="19"/>
+      <c r="D54" s="11"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="19"/>
+      <c r="D55" s="11"/>
+    </row>
+    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="D56" s="11"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="D57" s="11"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="D58" s="11"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="D59" s="11"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="4"/>
+      <c r="D60" s="11"/>
+    </row>
+    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="D61" s="11"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" s="21"/>
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" s="22"/>
+      <c r="D63" s="11"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="22"/>
+      <c r="D64" s="11"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="22"/>
+      <c r="D65" s="11"/>
+    </row>
+    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="23"/>
+      <c r="D66" s="11"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="D45" s="11"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="D46" s="11"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="D47" s="11"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="7"/>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="7"/>
-      <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B52" s="7"/>
-      <c r="D52" s="11"/>
+      <c r="B67" s="5"/>
+      <c r="D67" s="11"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="D68" s="11"/>
+    </row>
+    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B69" s="24"/>
+      <c r="D69" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1168,7 +1359,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E880C197-BC95-4C5B-A656-6C63E902724E}">
           <x14:formula1>
             <xm:f>Tabelle2!$A$2:$A$4</xm:f>
@@ -1191,13 +1382,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B28</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D34A55A2-833F-4BC2-A21D-77C18B0F6333}">
-          <x14:formula1>
-            <xm:f>Tabelle2!$I$2:$I$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B33</xm:sqref>
+          <xm:sqref>B28 B39 B43 B51:B52 B57 B62 B67 B33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1207,93 +1392,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A41E031-B515-4B55-B38F-F0D31894393C}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
       <c r="E7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Tabelle 'Privat_Krankenversicherte' mit entsprechenden Stored Procedures und Datenimport erfolgrich erstellt.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4B4FC5-2FCB-40DA-B4E4-8A4F41F8D3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F8A210-867A-4078-B385-D48961097CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -471,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -490,11 +490,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -780,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,29 +1128,37 @@
       <c r="A39" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="D39" s="11"/>
+      <c r="B39" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="D40" s="11"/>
+      <c r="B40" s="2">
+        <v>375.48</v>
+      </c>
+      <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="D41" s="11"/>
+      <c r="B41" s="2">
+        <v>37.549999999999997</v>
+      </c>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="D42" s="11"/>
+      <c r="B42" s="2">
+        <v>70</v>
+      </c>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
@@ -1163,52 +1168,52 @@
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
+      <c r="B44" s="5"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="18"/>
+      <c r="B45" s="5"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="18"/>
+      <c r="B46" s="5"/>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="18"/>
+      <c r="B47" s="5"/>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B48" s="18"/>
+      <c r="B48" s="5"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="18"/>
+      <c r="B49" s="5"/>
       <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="18"/>
+      <c r="B50" s="5"/>
       <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1219,38 +1224,38 @@
       <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="19"/>
+      <c r="B52" s="8"/>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="19"/>
+      <c r="B53" s="8"/>
       <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="19"/>
+      <c r="B54" s="8"/>
       <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="19"/>
+      <c r="B55" s="8"/>
       <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="20"/>
+      <c r="B56" s="18"/>
       <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1289,38 +1294,38 @@
       <c r="D61" s="11"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="21" t="s">
+      <c r="A62" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="21"/>
+      <c r="B62" s="19"/>
       <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="22"/>
+      <c r="B63" s="7"/>
       <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="22"/>
+      <c r="B64" s="7"/>
       <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="22" t="s">
+      <c r="A65" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="22"/>
+      <c r="B65" s="7"/>
       <c r="D65" s="11"/>
     </row>
     <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="23" t="s">
+      <c r="A66" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B66" s="23"/>
+      <c r="B66" s="20"/>
       <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1338,10 +1343,10 @@
       <c r="D68" s="11"/>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="24" t="s">
+      <c r="A69" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B69" s="24"/>
+      <c r="B69" s="21"/>
       <c r="D69" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabellen für 'gesetzliche KV-Beitraege' inkl. Stored Procedures und Datenimport erfolgreich erstellt. Aktueller Stand der BA eingefügt.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F8A210-867A-4078-B385-D48961097CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48300F3-E76F-4C52-B72C-D15D1E1AB765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1129,7 +1129,7 @@
         <v>101</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D39" s="10"/>
     </row>
@@ -1137,74 +1137,78 @@
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="2">
-        <v>375.48</v>
-      </c>
+      <c r="B40" s="2"/>
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="2">
-        <v>37.549999999999997</v>
-      </c>
+      <c r="B41" s="2"/>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="2">
-        <v>70</v>
-      </c>
+      <c r="B42" s="2"/>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="17"/>
+      <c r="B43" s="17" t="s">
+        <v>64</v>
+      </c>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="B44" s="5">
+        <v>7.3</v>
+      </c>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="B45" s="5">
+        <v>7.3</v>
+      </c>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="B46" s="5">
+        <v>72000</v>
+      </c>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="B47" s="5">
+        <v>68000</v>
+      </c>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="B48" s="5"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="B49" s="5"/>
       <c r="D49" s="11"/>

</xml_diff>

<commit_message>
Tabellen 'Krankenkassen', 'GKV_Zusatzbeitraege' und entsprechende Assoziationen + Stored Procedures und Datenimport erstellt. Läuft erfolgreich.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48300F3-E76F-4C52-B72C-D15D1E1AB765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF68CF6-68FE-4546-9767-CABDBFF1A2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -307,9 +307,6 @@
     <t>Risikoklasse Unfallversicherung</t>
   </si>
   <si>
-    <t>Zusatzbeitrag Krankenversicherung</t>
-  </si>
-  <si>
     <t>AG-Krankenversicherungsbeitrag in Prozent</t>
   </si>
   <si>
@@ -344,6 +341,15 @@
   </si>
   <si>
     <t>A5-1</t>
+  </si>
+  <si>
+    <t>KKH</t>
+  </si>
+  <si>
+    <t>Zusatzbeitrag Krankenversicherung in Prozent</t>
+  </si>
+  <si>
+    <t>Kaufmaennische Krankenkasse</t>
   </si>
 </sst>
 </file>
@@ -375,7 +381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,6 +436,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -471,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -494,6 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -777,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,7 +1097,7 @@
         <v>41</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34" s="10"/>
     </row>
@@ -1126,7 +1139,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>57</v>
@@ -1161,63 +1174,69 @@
       <c r="B43" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="11"/>
+      <c r="D43" s="22"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="5">
         <v>7.3</v>
       </c>
-      <c r="D44" s="11"/>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="5">
         <v>7.3</v>
       </c>
-      <c r="D45" s="11"/>
+      <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" s="5">
         <v>72000</v>
       </c>
-      <c r="D46" s="11"/>
+      <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="5">
         <v>68000</v>
       </c>
-      <c r="D47" s="11"/>
+      <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>105</v>
+      </c>
       <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1.5</v>
+      </c>
       <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1229,7 +1248,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" s="8"/>
       <c r="D52" s="11"/>
@@ -1243,21 +1262,21 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="8"/>
       <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" s="8"/>
       <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B56" s="18"/>
       <c r="D56" s="11"/>
@@ -1423,7 +1442,7 @@
         <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1483,7 +1502,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7">
         <v>6</v>

</xml_diff>

<commit_message>
Tabellen zu 'Anzahl Kinder bzw. AN-PV-BEitragssaetze' inkl. entsprechende Stored Procedures und Datenimports implementiert. Alles läuft erfolgreich.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF68CF6-68FE-4546-9767-CABDBFF1A2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCC743B-E8FA-46B3-AB5D-616D4D6EA6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -512,7 +512,98 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -523,6 +614,56 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7DC797-A95E-4482-8629-011774679158}" name="tbl_Geschlecht" displayName="tbl_Geschlecht" ref="A1:A4" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:A4" xr:uid="{9C7DC797-A95E-4482-8629-011774679158}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{F034D9B6-9D52-4274-B434-95E641979361}" name="Geschlecht"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D5ADE14-5AA7-4843-AE3B-15AFAD66EC57}" name="tbl_Mitarbeitertyp" displayName="tbl_Mitarbeitertyp" ref="C1:C7" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="C1:C7" xr:uid="{3D5ADE14-5AA7-4843-AE3B-15AFAD66EC57}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{FCF90F50-8B26-48B9-9CDC-1309BA948D07}" name="Mitarbeitertyp"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5720A5BB-2C5B-4A43-93CC-F04ADFC83CAE}" name="tbl_Steuerklasse" displayName="tbl_Steuerklasse" ref="E1:E7" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="E1:E7" xr:uid="{5720A5BB-2C5B-4A43-93CC-F04ADFC83CAE}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{51567C66-ECAC-455D-9A22-13EAF994E51B}" name="Steuerklasse"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F422A189-5D14-462B-BE76-5CC30C61C2C5}" name="tbl_ja_nein" displayName="tbl_ja_nein" ref="G1:G3" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="G1:G3" xr:uid="{F422A189-5D14-462B-BE76-5CC30C61C2C5}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{E96CACD0-03BA-4687-8818-6C96395A421D}" name="ja/nein"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{06875460-8491-4725-9779-5103659E4525}" name="tbl_Anzahl_Kinder" displayName="tbl_Anzahl_Kinder" ref="I1:I102" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="I1:I102" xr:uid="{06875460-8491-4725-9779-5103659E4525}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CAB87FE6-84F2-445A-98E2-61DBBA398E8A}" name="Anzahl Kinder"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -790,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,7 +1360,7 @@
       <c r="B48" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D48" s="11"/>
+      <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
@@ -1228,55 +1369,63 @@
       <c r="B49" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="10"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B50" s="5">
         <v>1.5</v>
       </c>
-      <c r="D50" s="11"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="17"/>
-      <c r="D51" s="11"/>
+      <c r="A51" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="8">
+        <v>2</v>
+      </c>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B52" s="8"/>
-      <c r="D52" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="B52" s="8">
+        <v>1</v>
+      </c>
+      <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53" s="8"/>
-      <c r="D53" s="11"/>
+        <v>98</v>
+      </c>
+      <c r="B53" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="D54" s="11"/>
+        <v>99</v>
+      </c>
+      <c r="B54" s="8">
+        <v>38000</v>
+      </c>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="B55" s="8"/>
       <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B56" s="18"/>
       <c r="D56" s="11"/>
@@ -1387,7 +1536,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E880C197-BC95-4C5B-A656-6C63E902724E}">
           <x14:formula1>
             <xm:f>Tabelle2!$A$2:$A$4</xm:f>
@@ -1410,7 +1559,13 @@
           <x14:formula1>
             <xm:f>Tabelle2!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B28 B39 B43 B51:B52 B57 B62 B67 B33</xm:sqref>
+          <xm:sqref>B28 B39 B43 B57 B62 B67 B33</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC540D61-4588-479B-B62B-BA6755FB2963}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$I$2:$I$102</xm:f>
+          </x14:formula1>
+          <xm:sqref>B51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1420,18 +1575,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A41E031-B515-4B55-B38F-F0D31894393C}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1444,8 +1602,11 @@
       <c r="G1" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1458,8 +1619,11 @@
       <c r="G2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1472,8 +1636,11 @@
       <c r="G3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1483,32 +1650,526 @@
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>62</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>63</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>102</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I78">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I80">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I91">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I93">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I94">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I95">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I97">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I98">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I99">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I100">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I101">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I102">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tabellen 'wohnhaft_Sachsen' bzw. 'AG_PV_Beitragssatz' inkl. Stored Procedures und Datenimport implementiert. Alle Tests und Programme laufen.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCC743B-E8FA-46B3-AB5D-616D4D6EA6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16492540-CE60-42E1-8F78-B4887E0450B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -1420,14 +1420,18 @@
       <c r="A55" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="8"/>
+      <c r="B55" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B56" s="18"/>
+      <c r="B56" s="18">
+        <v>1.2</v>
+      </c>
       <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1559,7 +1563,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B28 B39 B43 B57 B62 B67 B33</xm:sqref>
+          <xm:sqref>B28 B39 B43 B57 B62 B67 B33 B55</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC540D61-4588-479B-B62B-BA6755FB2963}">
           <x14:formula1>

</xml_diff>

<commit_message>
Tabellen für Bereich 'Arbeitslosenversicherung' inkl. Stored Procedures und dAtenimport erstellt. Alle Progammelaufen.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16492540-CE60-42E1-8F78-B4887E0450B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF157ECA-4664-4A8A-BB21-F6901F9A3C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37305" yWindow="2625" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -356,7 +356,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,8 +380,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,12 +442,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -483,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -506,7 +506,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -931,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,7 +1321,7 @@
       <c r="B43" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="22"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
@@ -1423,7 +1429,7 @@
       <c r="B55" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="11"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
@@ -1432,97 +1438,107 @@
       <c r="B56" s="18">
         <v>1.2</v>
       </c>
-      <c r="D56" s="11"/>
+      <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="3"/>
-      <c r="D57" s="11"/>
+      <c r="B57" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="10"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="D58" s="11"/>
+      <c r="B58" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="D58" s="10"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B59" s="4"/>
-      <c r="D59" s="11"/>
+      <c r="B59" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="D59" s="10"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B60" s="4"/>
-      <c r="D60" s="11"/>
+      <c r="B60" s="22">
+        <v>64123</v>
+      </c>
+      <c r="D60" s="10"/>
     </row>
     <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B61" s="3"/>
-      <c r="D61" s="11"/>
+      <c r="B61" s="23">
+        <v>68543</v>
+      </c>
+      <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="19"/>
+      <c r="B62" s="24"/>
       <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="7"/>
+      <c r="B63" s="25"/>
       <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="7"/>
+      <c r="B64" s="25"/>
       <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="7"/>
+      <c r="B65" s="25"/>
       <c r="D65" s="11"/>
     </row>
     <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B66" s="20"/>
+      <c r="B66" s="26"/>
       <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B67" s="5"/>
+      <c r="B67" s="27"/>
       <c r="D67" s="11"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="5"/>
+      <c r="B68" s="27"/>
       <c r="D68" s="11"/>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B69" s="21"/>
+      <c r="B69" s="28"/>
       <c r="D69" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabellen, stored Procedures und Datenimport für Bereich 'Rentenversicherung' erstellt. Alle Tests laufen erfolgreich.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
+++ b/src/main/Mitarbeiterdaten/Max Mustermann.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF157ECA-4664-4A8A-BB21-F6901F9A3C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DE59D9-74C2-4714-B298-4556F7EB37C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37305" yWindow="2625" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="108">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,35 +1489,45 @@
       <c r="A62" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="24"/>
+      <c r="B62" s="24" t="s">
+        <v>64</v>
+      </c>
       <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="25"/>
+      <c r="B63" s="25">
+        <v>10.3</v>
+      </c>
       <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="25"/>
+      <c r="B64" s="25">
+        <v>10.3</v>
+      </c>
       <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="25"/>
+      <c r="B65" s="25">
+        <v>78563.45</v>
+      </c>
       <c r="D65" s="11"/>
     </row>
     <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B66" s="26"/>
+      <c r="B66" s="26">
+        <v>81253</v>
+      </c>
       <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>